<commit_message>
Added TC005 and TC006
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -1,37 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFAB8ED9-1BC6-44E1-A66F-92F4238171AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SohailShaikhFaiyaz\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
+    <sheet name="tc005" sheetId="2" r:id="rId2"/>
+    <sheet name="tc006" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>STG- PulseCodeOnAzureCloud</t>
+  </si>
+  <si>
+    <t>Epic name</t>
+  </si>
+  <si>
+    <t>Epic 039</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -50,13 +56,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -69,14 +69,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -85,10 +77,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -257,6 +249,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -283,24 +276,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -361,50 +355,81 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TC009 and TC010 commit
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFAB8ED9-1BC6-44E1-A66F-92F4238171AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="6200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
+    <sheet name="tc009" sheetId="2" r:id="rId2"/>
+    <sheet name="tc010" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -30,26 +28,400 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>epic</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>reqId</t>
+  </si>
+  <si>
+    <t>STG- PulseCodeOnAzureCloud</t>
+  </si>
+  <si>
+    <t>Epic 039</t>
+  </si>
+  <si>
+    <t>feature 039</t>
+  </si>
+  <si>
+    <t>RQ-24</t>
+  </si>
+  <si>
+    <t>moduleId</t>
+  </si>
+  <si>
+    <t>RQF 12</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -57,24 +429,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -123,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -156,26 +814,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -208,23 +849,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -386,25 +1010,126 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="30.4166666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="13.0833333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="31.1666666666667" customWidth="1"/>
+    <col min="3" max="3" width="14.4166666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TC017 and TC018 commit
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -1,29 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\TestNext Release 2\testData\requirementTabTestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF4EAC-1377-4027-8ABF-48B991EF2176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
     <sheet name="tc002" sheetId="3" r:id="rId2"/>
     <sheet name="tc011" sheetId="4" r:id="rId3"/>
     <sheet name="tc012" sheetId="5" r:id="rId4"/>
+    <sheet name="tc010" sheetId="7" r:id="rId5"/>
+    <sheet name="tc017" sheetId="8" r:id="rId6"/>
+    <sheet name="naa" sheetId="9" r:id="rId7"/>
+    <sheet name="tc018" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>Project Name</t>
   </si>
@@ -67,31 +78,77 @@
     <t>Rq</t>
   </si>
   <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>pri1</t>
+  </si>
+  <si>
     <t>RQ-463</t>
   </si>
   <si>
-    <t>priority</t>
-  </si>
-  <si>
     <t>Must have</t>
   </si>
   <si>
-    <t>pri1</t>
-  </si>
-  <si>
     <t>Should have</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>epic</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>moduleId</t>
+  </si>
+  <si>
+    <t>Epic 039</t>
+  </si>
+  <si>
+    <t>feature 039</t>
+  </si>
+  <si>
+    <t>RQF 12</t>
+  </si>
+  <si>
+    <t>feature 7</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>descri</t>
+  </si>
+  <si>
+    <t>Module 25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -100,16 +157,346 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -117,25 +504,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -413,25 +1087,25 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+    <col min="1" max="1" width="32.725" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.90625" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.9083333333333" customWidth="1"/>
+    <col min="4" max="4" width="17.3666666666667" customWidth="1"/>
+    <col min="5" max="5" width="18.2666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -464,27 +1138,29 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" customWidth="1"/>
+    <col min="3" max="3" width="16.1833333333333" customWidth="1"/>
+    <col min="4" max="4" width="24.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -517,23 +1193,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018D6FBF-87E3-4965-9926-26DA875C70B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="28.08984375" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.0916666666667" customWidth="1"/>
+    <col min="2" max="2" width="15.1833333333333" customWidth="1"/>
+    <col min="4" max="4" width="11.1833333333333" customWidth="1"/>
+    <col min="5" max="5" width="14.5416666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -547,10 +1225,10 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -561,10 +1239,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -572,22 +1250,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A98A44B-A0FA-45FE-9B5B-68B8C5758F74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="16.9083333333333" customWidth="1"/>
+    <col min="3" max="3" width="15.9083333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -609,10 +1289,211 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="3" max="3" width="13.1666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="30.9166666666667" customWidth="1"/>
+    <col min="2" max="2" width="19.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="31.5833333333333" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="11.8333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Few bugs fixed for tc026,tc028,tc037,tc018,tc025,tc037
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="8" activeTab="12"/>
+    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="tc033" sheetId="22" r:id="rId27"/>
     <sheet name="tc004" sheetId="13" r:id="rId28"/>
     <sheet name="tc019" sheetId="12" r:id="rId29"/>
+    <sheet name="tc036" sheetId="30" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="68">
   <si>
     <t>Project Name</t>
   </si>
@@ -193,9 +194,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Module 123</t>
   </si>
   <si>
     <t>Rqname</t>
@@ -1359,7 +1357,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1475,8 +1473,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1556,8 +1554,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.8583333333333" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1575,10 +1573,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +1664,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>32</v>
@@ -1723,19 +1721,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1746,13 +1744,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1774,16 +1772,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1794,10 +1792,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1877,13 +1875,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1894,7 +1892,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1909,26 +1907,26 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1939,10 +1937,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
@@ -1967,16 +1965,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1987,10 +1985,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2012,16 +2010,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2032,7 +2030,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>22</v>
@@ -2087,7 +2085,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2146,7 +2144,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2181,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +2203,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -2213,7 +2211,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -2247,7 +2245,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2258,10 +2256,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2299,6 +2297,39 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2491,7 +2522,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
suite ran successfully and report added for requirement
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="14" activeTab="14"/>
+    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="69">
   <si>
     <t>Project Name</t>
   </si>
@@ -100,36 +100,42 @@
     <t>pri1</t>
   </si>
   <si>
+    <t>Epic 039</t>
+  </si>
+  <si>
+    <t>RQ-443</t>
+  </si>
+  <si>
+    <t>Must have</t>
+  </si>
+  <si>
+    <t>Should have</t>
+  </si>
+  <si>
+    <t>Rq1</t>
+  </si>
+  <si>
+    <t>c_desc</t>
+  </si>
+  <si>
+    <t>Rq12</t>
+  </si>
+  <si>
+    <t>RQ-466</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>hi,this is description</t>
+  </si>
+  <si>
     <t>RQ-463</t>
   </si>
   <si>
-    <t>Must have</t>
-  </si>
-  <si>
-    <t>Should have</t>
-  </si>
-  <si>
-    <t>Rq1</t>
-  </si>
-  <si>
-    <t>c_desc</t>
-  </si>
-  <si>
-    <t>Rq12</t>
-  </si>
-  <si>
-    <t>RQ-466</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>hi,this is description</t>
-  </si>
-  <si>
     <t>ProjectName</t>
   </si>
   <si>
@@ -137,9 +143,6 @@
   </si>
   <si>
     <t>moduleName</t>
-  </si>
-  <si>
-    <t>Epic 039</t>
   </si>
   <si>
     <t>Epic 2</t>
@@ -1313,7 +1316,58 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -1327,79 +1381,28 @@
       <c r="E1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="F2" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1424,42 +1427,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1486,13 +1489,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1500,10 +1503,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1529,10 +1532,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1540,7 +1543,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1554,8 +1557,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.8583333333333" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1565,10 +1568,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1576,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1604,16 +1607,16 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1621,19 +1624,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1664,19 +1667,19 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1684,22 +1687,22 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1721,19 +1724,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1741,16 +1744,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1772,16 +1775,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1789,13 +1792,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1809,8 +1812,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1844,16 +1847,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1875,13 +1878,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1889,10 +1892,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1914,19 +1917,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1934,16 +1937,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1965,16 +1968,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1982,13 +1985,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2010,16 +2013,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2027,13 +2030,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2048,7 +2051,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2059,10 +2062,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2096,10 +2099,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2107,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2133,10 +2136,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2144,7 +2147,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2170,10 +2173,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2181,7 +2184,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2203,18 +2206,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2242,10 +2245,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2256,10 +2259,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2314,10 +2317,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2325,7 +2328,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2356,13 +2359,13 @@
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2373,16 +2376,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2413,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2427,7 +2430,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2477,7 +2480,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2502,7 +2505,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -2533,10 +2536,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2544,7 +2547,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2577,10 +2580,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2591,10 +2594,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few minor code updated for landing page test plan
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -1302,8 +1302,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1812,8 +1812,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>

</xml_diff>